<commit_message>
Enable crawler start from stored DB
</commit_message>
<xml_diff>
--- a/analysis/analysis.xlsx
+++ b/analysis/analysis.xlsx
@@ -571,7 +571,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -985,7 +984,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Max Conn = 2</c:v>
+            <c:v>Max Conn = 10</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1109,7 +1108,7 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Max Conn = 3</c:v>
+            <c:v>Max Conn = 100</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -6232,8 +6231,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K75" sqref="K75"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6328,7 +6327,7 @@
         <v>3018</v>
       </c>
       <c r="I3">
-        <f>F3/G3</f>
+        <f t="shared" ref="I3:I32" si="0">F3/G3</f>
         <v>0.17064280980781976</v>
       </c>
       <c r="K3">
@@ -6338,7 +6337,7 @@
         <v>3318</v>
       </c>
       <c r="N3">
-        <f>K3/L3</f>
+        <f t="shared" ref="N3:N32" si="1">K3/L3</f>
         <v>0.16335141651597349</v>
       </c>
     </row>
@@ -6354,7 +6353,7 @@
         <v>93</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D32" si="0">A4/B4</f>
+        <f t="shared" ref="D4:D32" si="2">A4/B4</f>
         <v>0.11402946828955797</v>
       </c>
       <c r="F4">
@@ -6364,11 +6363,11 @@
         <v>5792</v>
       </c>
       <c r="H4">
-        <f>F4-F3</f>
+        <f t="shared" ref="H4:H32" si="3">F4-F3</f>
         <v>1095</v>
       </c>
       <c r="I4">
-        <f>F4/G4</f>
+        <f t="shared" si="0"/>
         <v>0.27796961325966851</v>
       </c>
       <c r="K4">
@@ -6378,11 +6377,11 @@
         <v>5983</v>
       </c>
       <c r="M4">
-        <f>K4-K3</f>
+        <f t="shared" ref="M4:M32" si="4">K4-K3</f>
         <v>1230</v>
       </c>
       <c r="N4">
-        <f>K4/L4</f>
+        <f t="shared" si="1"/>
         <v>0.29617248871803442</v>
       </c>
     </row>
@@ -6394,11 +6393,11 @@
         <v>1745</v>
       </c>
       <c r="C5">
-        <f t="shared" ref="C5:C32" si="1">A5-A4</f>
+        <f t="shared" ref="C5:C32" si="5">A5-A4</f>
         <v>78</v>
       </c>
       <c r="D5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.14670487106017191</v>
       </c>
       <c r="F5">
@@ -6408,11 +6407,11 @@
         <v>8528</v>
       </c>
       <c r="H5">
-        <f>F5-F4</f>
+        <f t="shared" si="3"/>
         <v>882</v>
       </c>
       <c r="I5">
-        <f>F5/G5</f>
+        <f t="shared" si="0"/>
         <v>0.29221388367729834</v>
       </c>
       <c r="K5">
@@ -6422,11 +6421,11 @@
         <v>8470</v>
       </c>
       <c r="M5">
-        <f>K5-K4</f>
+        <f t="shared" si="4"/>
         <v>927</v>
       </c>
       <c r="N5">
-        <f>K5/L5</f>
+        <f t="shared" si="1"/>
         <v>0.31865407319952777</v>
       </c>
     </row>
@@ -6438,11 +6437,11 @@
         <v>1767</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
       <c r="D6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.155631013016412</v>
       </c>
       <c r="F6">
@@ -6452,11 +6451,11 @@
         <v>10304</v>
       </c>
       <c r="H6">
-        <f>F6-F5</f>
+        <f t="shared" si="3"/>
         <v>732</v>
       </c>
       <c r="I6">
-        <f>F6/G6</f>
+        <f t="shared" si="0"/>
         <v>0.31288819875776397</v>
       </c>
       <c r="K6">
@@ -6466,11 +6465,11 @@
         <v>9887</v>
       </c>
       <c r="M6">
-        <f>K6-K5</f>
+        <f t="shared" si="4"/>
         <v>439</v>
       </c>
       <c r="N6">
-        <f>K6/L6</f>
+        <f t="shared" si="1"/>
         <v>0.31738646707798118</v>
       </c>
     </row>
@@ -6482,11 +6481,11 @@
         <v>1775</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.1571830985915493</v>
       </c>
       <c r="F7">
@@ -6496,11 +6495,11 @@
         <v>11001</v>
       </c>
       <c r="H7">
-        <f>F7-F6</f>
+        <f t="shared" si="3"/>
         <v>310</v>
       </c>
       <c r="I7">
-        <f>F7/G7</f>
+        <f t="shared" si="0"/>
         <v>0.32124352331606215</v>
       </c>
       <c r="K7">
@@ -6510,11 +6509,11 @@
         <v>10616</v>
       </c>
       <c r="M7">
-        <f>K7-K6</f>
+        <f t="shared" si="4"/>
         <v>353</v>
       </c>
       <c r="N7">
-        <f>K7/L7</f>
+        <f t="shared" si="1"/>
         <v>0.32884325546345139</v>
       </c>
     </row>
@@ -6526,11 +6525,11 @@
         <v>1782</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.15993265993265993</v>
       </c>
       <c r="F8">
@@ -6540,11 +6539,11 @@
         <v>11114</v>
       </c>
       <c r="H8">
-        <f>F8-F7</f>
+        <f t="shared" si="3"/>
         <v>364</v>
       </c>
       <c r="I8">
-        <f>F8/G8</f>
+        <f t="shared" si="0"/>
         <v>0.35072881050926757</v>
       </c>
       <c r="K8">
@@ -6554,11 +6553,11 @@
         <v>10725</v>
       </c>
       <c r="M8">
-        <f>K8-K7</f>
+        <f t="shared" si="4"/>
         <v>285</v>
       </c>
       <c r="N8">
-        <f>K8/L8</f>
+        <f t="shared" si="1"/>
         <v>0.35207459207459207</v>
       </c>
     </row>
@@ -6570,11 +6569,11 @@
         <v>1785</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16190476190476191</v>
       </c>
       <c r="F9">
@@ -6584,11 +6583,11 @@
         <v>12219</v>
       </c>
       <c r="H9">
-        <f>F9-F8</f>
+        <f t="shared" si="3"/>
         <v>519</v>
       </c>
       <c r="I9">
-        <f>F9/G9</f>
+        <f t="shared" si="0"/>
         <v>0.36148621000081838</v>
       </c>
       <c r="K9">
@@ -6598,11 +6597,11 @@
         <v>12506</v>
       </c>
       <c r="M9">
-        <f>K9-K8</f>
+        <f t="shared" si="4"/>
         <v>762</v>
       </c>
       <c r="N9">
-        <f>K9/L9</f>
+        <f t="shared" si="1"/>
         <v>0.36286582440428594</v>
       </c>
     </row>
@@ -6614,11 +6613,11 @@
         <v>1795</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16545961002785514</v>
       </c>
       <c r="F10">
@@ -6628,11 +6627,11 @@
         <v>14545</v>
       </c>
       <c r="H10">
-        <f>F10-F9</f>
+        <f t="shared" si="3"/>
         <v>682</v>
       </c>
       <c r="I10">
-        <f>F10/G10</f>
+        <f t="shared" si="0"/>
         <v>0.35056720522516327</v>
       </c>
       <c r="K10">
@@ -6642,11 +6641,11 @@
         <v>14227</v>
       </c>
       <c r="M10">
-        <f>K10-K9</f>
+        <f t="shared" si="4"/>
         <v>1165</v>
       </c>
       <c r="N10">
-        <f>K10/L10</f>
+        <f t="shared" si="1"/>
         <v>0.40085752442538836</v>
       </c>
     </row>
@@ -6658,11 +6657,11 @@
         <v>1946</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>21</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16341212744090441</v>
       </c>
       <c r="F11">
@@ -6672,11 +6671,11 @@
         <v>15544</v>
       </c>
       <c r="H11">
-        <f>F11-F10</f>
+        <f t="shared" si="3"/>
         <v>846</v>
       </c>
       <c r="I11">
-        <f>F11/G11</f>
+        <f t="shared" si="0"/>
         <v>0.3824626865671642</v>
       </c>
       <c r="K11">
@@ -6686,11 +6685,11 @@
         <v>18737</v>
       </c>
       <c r="M11">
-        <f>K11-K10</f>
+        <f t="shared" si="4"/>
         <v>1169</v>
       </c>
       <c r="N11">
-        <f>K11/L11</f>
+        <f t="shared" si="1"/>
         <v>0.36676095426162136</v>
       </c>
     </row>
@@ -6702,11 +6701,11 @@
         <v>1955</v>
       </c>
       <c r="C12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.16982097186700768</v>
       </c>
       <c r="F12">
@@ -6716,11 +6715,11 @@
         <v>16059</v>
       </c>
       <c r="H12">
-        <f>F12-F11</f>
+        <f t="shared" si="3"/>
         <v>150</v>
       </c>
       <c r="I12">
-        <f>F12/G12</f>
+        <f t="shared" si="0"/>
         <v>0.37953795379537952</v>
       </c>
       <c r="K12">
@@ -6730,11 +6729,11 @@
         <v>19072</v>
       </c>
       <c r="M12">
-        <f>K12-K11</f>
+        <f t="shared" si="4"/>
         <v>921</v>
       </c>
       <c r="N12">
-        <f>K12/L12</f>
+        <f t="shared" si="1"/>
         <v>0.40860947986577179</v>
       </c>
     </row>
@@ -6746,11 +6745,11 @@
         <v>1971</v>
       </c>
       <c r="C13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.17757483510908167</v>
       </c>
       <c r="F13">
@@ -6760,11 +6759,11 @@
         <v>16359</v>
       </c>
       <c r="H13">
-        <f>F13-F12</f>
+        <f t="shared" si="3"/>
         <v>109</v>
       </c>
       <c r="I13">
-        <f>F13/G13</f>
+        <f t="shared" si="0"/>
         <v>0.37924078488905189</v>
       </c>
       <c r="K13">
@@ -6774,11 +6773,11 @@
         <v>22044</v>
       </c>
       <c r="M13">
-        <f>K13-K12</f>
+        <f t="shared" si="4"/>
         <v>1281</v>
       </c>
       <c r="N13">
-        <f>K13/L13</f>
+        <f t="shared" si="1"/>
         <v>0.41163128288876794</v>
       </c>
     </row>
@@ -6790,11 +6789,11 @@
         <v>2002</v>
       </c>
       <c r="C14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18381618381618381</v>
       </c>
       <c r="F14">
@@ -6804,11 +6803,11 @@
         <v>16596</v>
       </c>
       <c r="H14">
-        <f>F14-F13</f>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
       <c r="I14">
-        <f>F14/G14</f>
+        <f t="shared" si="0"/>
         <v>0.37858520125331407</v>
       </c>
       <c r="K14">
@@ -6818,11 +6817,11 @@
         <v>24070</v>
       </c>
       <c r="M14">
-        <f>K14-K13</f>
+        <f t="shared" si="4"/>
         <v>526</v>
       </c>
       <c r="N14">
-        <f>K14/L14</f>
+        <f t="shared" si="1"/>
         <v>0.39883672621520566</v>
       </c>
     </row>
@@ -6834,11 +6833,11 @@
         <v>2358</v>
       </c>
       <c r="C15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>100</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19847328244274809</v>
       </c>
       <c r="F15">
@@ -6848,11 +6847,11 @@
         <v>16722</v>
       </c>
       <c r="H15">
-        <f>F15-F14</f>
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
       <c r="I15">
-        <f>F15/G15</f>
+        <f t="shared" si="0"/>
         <v>0.37991867001554835</v>
       </c>
       <c r="K15">
@@ -6862,11 +6861,11 @@
         <v>24072</v>
       </c>
       <c r="M15">
-        <f>K15-K14</f>
+        <f t="shared" si="4"/>
         <v>216</v>
       </c>
       <c r="N15">
-        <f>K15/L15</f>
+        <f t="shared" si="1"/>
         <v>0.40777666999002993</v>
       </c>
     </row>
@@ -6878,11 +6877,11 @@
         <v>2809</v>
       </c>
       <c r="C16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>45</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18262726949092203</v>
       </c>
       <c r="F16">
@@ -6892,11 +6891,11 @@
         <v>16989</v>
       </c>
       <c r="H16">
-        <f>F16-F15</f>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
       <c r="I16">
-        <f>F16/G16</f>
+        <f t="shared" si="0"/>
         <v>0.37906880922950142</v>
       </c>
       <c r="K16">
@@ -6906,11 +6905,11 @@
         <v>33079</v>
       </c>
       <c r="M16">
-        <f>K16-K15</f>
+        <f t="shared" si="4"/>
         <v>1071</v>
       </c>
       <c r="N16">
-        <f>K16/L16</f>
+        <f t="shared" si="1"/>
         <v>0.32912119471568063</v>
       </c>
     </row>
@@ -6922,11 +6921,11 @@
         <v>2889</v>
       </c>
       <c r="C17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>34</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.18933887158186224</v>
       </c>
       <c r="F17">
@@ -6936,11 +6935,11 @@
         <v>17372</v>
       </c>
       <c r="H17">
-        <f>F17-F16</f>
+        <f t="shared" si="3"/>
         <v>111</v>
       </c>
       <c r="I17">
-        <f>F17/G17</f>
+        <f t="shared" si="0"/>
         <v>0.37710108220124339</v>
       </c>
       <c r="K17">
@@ -6950,11 +6949,11 @@
         <v>33933</v>
       </c>
       <c r="M17">
-        <f>K17-K16</f>
+        <f t="shared" si="4"/>
         <v>352</v>
       </c>
       <c r="N17">
-        <f>K17/L17</f>
+        <f t="shared" si="1"/>
         <v>0.33121150502460733</v>
       </c>
     </row>
@@ -6966,11 +6965,11 @@
         <v>3007</v>
       </c>
       <c r="C18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>44</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19654140339208515</v>
       </c>
       <c r="F18">
@@ -6980,11 +6979,11 @@
         <v>17917</v>
       </c>
       <c r="H18">
-        <f>F18-F17</f>
+        <f t="shared" si="3"/>
         <v>149</v>
       </c>
       <c r="I18">
-        <f>F18/G18</f>
+        <f t="shared" si="0"/>
         <v>0.37394653122732602</v>
       </c>
       <c r="K18">
@@ -6994,11 +6993,11 @@
         <v>33933</v>
       </c>
       <c r="M18">
-        <f>K18-K17</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N18">
-        <f>K18/L18</f>
+        <f t="shared" si="1"/>
         <v>0.33121150502460733</v>
       </c>
     </row>
@@ -7010,11 +7009,11 @@
         <v>3047</v>
       </c>
       <c r="C19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.19855595667870035</v>
       </c>
       <c r="F19">
@@ -7024,11 +7023,11 @@
         <v>18535</v>
       </c>
       <c r="H19">
-        <f>F19-F18</f>
+        <f t="shared" si="3"/>
         <v>248</v>
       </c>
       <c r="I19">
-        <f>F19/G19</f>
+        <f t="shared" si="0"/>
         <v>0.37485837604531969</v>
       </c>
       <c r="K19">
@@ -7038,11 +7037,11 @@
         <v>33933</v>
       </c>
       <c r="M19">
-        <f>K19-K18</f>
+        <f t="shared" si="4"/>
         <v>108</v>
       </c>
       <c r="N19">
-        <f>K19/L19</f>
+        <f t="shared" si="1"/>
         <v>0.33439424748769636</v>
       </c>
     </row>
@@ -7054,11 +7053,11 @@
         <v>3452</v>
       </c>
       <c r="C20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>90</v>
       </c>
       <c r="D20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.20133256083429896</v>
       </c>
       <c r="F20">
@@ -7068,11 +7067,11 @@
         <v>19500</v>
       </c>
       <c r="H20">
-        <f>F20-F19</f>
+        <f t="shared" si="3"/>
         <v>307</v>
       </c>
       <c r="I20">
-        <f>F20/G20</f>
+        <f t="shared" si="0"/>
         <v>0.37205128205128207</v>
       </c>
       <c r="K20">
@@ -7082,11 +7081,11 @@
         <v>35384</v>
       </c>
       <c r="M20">
-        <f>K20-K19</f>
+        <f t="shared" si="4"/>
         <v>357</v>
       </c>
       <c r="N20">
-        <f>K20/L20</f>
+        <f t="shared" si="1"/>
         <v>0.33077096992991184</v>
       </c>
     </row>
@@ -7098,11 +7097,11 @@
         <v>4053</v>
       </c>
       <c r="C21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>231</v>
       </c>
       <c r="D21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.22847273624475697</v>
       </c>
       <c r="F21">
@@ -7112,11 +7111,11 @@
         <v>20229</v>
       </c>
       <c r="H21">
-        <f>F21-F20</f>
+        <f t="shared" si="3"/>
         <v>366</v>
       </c>
       <c r="I21">
-        <f>F21/G21</f>
+        <f t="shared" si="0"/>
         <v>0.37673636857976173</v>
       </c>
       <c r="K21">
@@ -7126,11 +7125,11 @@
         <v>36834</v>
       </c>
       <c r="M21">
-        <f>K21-K20</f>
+        <f t="shared" si="4"/>
         <v>1158</v>
       </c>
       <c r="N21">
-        <f>K21/L21</f>
+        <f t="shared" si="1"/>
         <v>0.34918824998642556</v>
       </c>
     </row>
@@ -7142,11 +7141,11 @@
         <v>4619</v>
       </c>
       <c r="C22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>301</v>
       </c>
       <c r="D22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.26564191383416325</v>
       </c>
       <c r="F22">
@@ -7156,11 +7155,11 @@
         <v>20365</v>
       </c>
       <c r="H22">
-        <f>F22-F21</f>
+        <f t="shared" si="3"/>
         <v>292</v>
       </c>
       <c r="I22">
-        <f>F22/G22</f>
+        <f t="shared" si="0"/>
         <v>0.38855880186594649</v>
       </c>
       <c r="K22">
@@ -7170,11 +7169,11 @@
         <v>37365</v>
       </c>
       <c r="M22">
-        <f>K22-K21</f>
+        <f t="shared" si="4"/>
         <v>414</v>
       </c>
       <c r="N22">
-        <f>K22/L22</f>
+        <f t="shared" si="1"/>
         <v>0.35530576742941256</v>
       </c>
     </row>
@@ -7186,11 +7185,11 @@
         <v>4983</v>
       </c>
       <c r="C23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>177</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28175797712221551</v>
       </c>
       <c r="F23">
@@ -7200,11 +7199,11 @@
         <v>20364</v>
       </c>
       <c r="H23">
-        <f>F23-F22</f>
+        <f t="shared" si="3"/>
         <v>197</v>
       </c>
       <c r="I23">
-        <f>F23/G23</f>
+        <f t="shared" si="0"/>
         <v>0.39825181693184053</v>
       </c>
       <c r="K23">
@@ -7214,11 +7213,11 @@
         <v>37678</v>
       </c>
       <c r="M23">
-        <f>K23-K22</f>
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
       <c r="N23">
-        <f>K23/L23</f>
+        <f t="shared" si="1"/>
         <v>0.36031636498752589</v>
       </c>
     </row>
@@ -7230,11 +7229,11 @@
         <v>4990</v>
       </c>
       <c r="C24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
       <c r="D24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28316633266533064</v>
       </c>
       <c r="F24">
@@ -7244,11 +7243,11 @@
         <v>20369</v>
       </c>
       <c r="H24">
-        <f>F24-F23</f>
+        <f t="shared" si="3"/>
         <v>278</v>
       </c>
       <c r="I24">
-        <f>F24/G24</f>
+        <f t="shared" si="0"/>
         <v>0.4118022485149001</v>
       </c>
       <c r="K24">
@@ -7258,11 +7257,11 @@
         <v>37881</v>
       </c>
       <c r="M24">
-        <f>K24-K23</f>
+        <f t="shared" si="4"/>
         <v>94</v>
       </c>
       <c r="N24">
-        <f>K24/L24</f>
+        <f t="shared" si="1"/>
         <v>0.36086692537155829</v>
       </c>
     </row>
@@ -7274,11 +7273,11 @@
         <v>5000</v>
       </c>
       <c r="C25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28360000000000002</v>
       </c>
       <c r="F25">
@@ -7288,11 +7287,11 @@
         <v>21208</v>
       </c>
       <c r="H25">
-        <f>F25-F24</f>
+        <f t="shared" si="3"/>
         <v>622</v>
       </c>
       <c r="I25">
-        <f>F25/G25</f>
+        <f t="shared" si="0"/>
         <v>0.42483968313843834</v>
       </c>
       <c r="K25">
@@ -7302,11 +7301,11 @@
         <v>38804</v>
       </c>
       <c r="M25">
-        <f>K25-K24</f>
+        <f t="shared" si="4"/>
         <v>194</v>
       </c>
       <c r="N25">
-        <f>K25/L25</f>
+        <f t="shared" si="1"/>
         <v>0.35728275435522111</v>
       </c>
     </row>
@@ -7318,11 +7317,11 @@
         <v>5012</v>
       </c>
       <c r="C26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28391859537110936</v>
       </c>
       <c r="F26">
@@ -7332,11 +7331,11 @@
         <v>23570</v>
       </c>
       <c r="H26">
-        <f>F26-F25</f>
+        <f t="shared" si="3"/>
         <v>603</v>
       </c>
       <c r="I26">
-        <f>F26/G26</f>
+        <f t="shared" si="0"/>
         <v>0.40784896054306324</v>
       </c>
       <c r="K26">
@@ -7346,11 +7345,11 @@
         <v>38804</v>
       </c>
       <c r="M26">
-        <f>K26-K25</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="N26">
-        <f>K26/L26</f>
+        <f t="shared" si="1"/>
         <v>0.35728275435522111</v>
       </c>
     </row>
@@ -7362,11 +7361,11 @@
         <v>5017</v>
       </c>
       <c r="C27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="D27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28463225034881401</v>
       </c>
       <c r="F27">
@@ -7376,11 +7375,11 @@
         <v>25566</v>
       </c>
       <c r="H27">
-        <f>F27-F26</f>
+        <f t="shared" si="3"/>
         <v>824</v>
       </c>
       <c r="I27">
-        <f>F27/G27</f>
+        <f t="shared" si="0"/>
         <v>0.40823750293358368</v>
       </c>
       <c r="K27">
@@ -7390,11 +7389,11 @@
         <v>39712</v>
       </c>
       <c r="M27">
-        <f>K27-K26</f>
+        <f t="shared" si="4"/>
         <v>173</v>
       </c>
       <c r="N27">
-        <f>K27/L27</f>
+        <f t="shared" si="1"/>
         <v>0.35346998388396456</v>
       </c>
     </row>
@@ -7406,11 +7405,11 @@
         <v>5017</v>
       </c>
       <c r="C28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28523021726131154</v>
       </c>
       <c r="F28">
@@ -7420,11 +7419,11 @@
         <v>26664</v>
       </c>
       <c r="H28">
-        <f>F28-F27</f>
+        <f t="shared" si="3"/>
         <v>836</v>
       </c>
       <c r="I28">
-        <f>F28/G28</f>
+        <f t="shared" si="0"/>
         <v>0.42277977797779775</v>
       </c>
       <c r="K28">
@@ -7434,11 +7433,11 @@
         <v>40041</v>
       </c>
       <c r="M28">
-        <f>K28-K27</f>
+        <f t="shared" si="4"/>
         <v>60</v>
       </c>
       <c r="N28">
-        <f>K28/L28</f>
+        <f t="shared" si="1"/>
         <v>0.35206413426238103</v>
       </c>
     </row>
@@ -7450,11 +7449,11 @@
         <v>5021</v>
       </c>
       <c r="C29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
       <c r="D29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28560047799243177</v>
       </c>
       <c r="F29">
@@ -7464,11 +7463,11 @@
         <v>27821</v>
       </c>
       <c r="H29">
-        <f>F29-F28</f>
+        <f t="shared" si="3"/>
         <v>283</v>
       </c>
       <c r="I29">
-        <f>F29/G29</f>
+        <f t="shared" si="0"/>
         <v>0.41536968477049713</v>
       </c>
       <c r="K29">
@@ -7478,11 +7477,11 @@
         <v>35736</v>
       </c>
       <c r="M29">
-        <f>K29-K28</f>
+        <f t="shared" si="4"/>
         <v>217</v>
       </c>
       <c r="N29">
-        <f>K29/L29</f>
+        <f t="shared" si="1"/>
         <v>0.40054846653234832</v>
       </c>
     </row>
@@ -7494,11 +7493,11 @@
         <v>5021</v>
       </c>
       <c r="C30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28579964150567616</v>
       </c>
       <c r="F30">
@@ -7508,11 +7507,11 @@
         <v>27837</v>
       </c>
       <c r="H30">
-        <f>F30-F29</f>
+        <f t="shared" si="3"/>
         <v>35</v>
       </c>
       <c r="I30">
-        <f>F30/G30</f>
+        <f t="shared" si="0"/>
         <v>0.41638826022919134</v>
       </c>
       <c r="K30">
@@ -7522,11 +7521,11 @@
         <v>40728</v>
       </c>
       <c r="M30">
-        <f>K30-K29</f>
+        <f t="shared" si="4"/>
         <v>261</v>
       </c>
       <c r="N30">
-        <f>K30/L30</f>
+        <f t="shared" si="1"/>
         <v>0.35786191318012178</v>
       </c>
     </row>
@@ -7538,11 +7537,11 @@
         <v>5040</v>
       </c>
       <c r="C31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="D31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28630952380952379</v>
       </c>
       <c r="F31">
@@ -7552,11 +7551,11 @@
         <v>28098</v>
       </c>
       <c r="H31">
-        <f>F31-F30</f>
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
       <c r="I31">
-        <f>F31/G31</f>
+        <f t="shared" si="0"/>
         <v>0.41508292405153391</v>
       </c>
       <c r="K31">
@@ -7566,11 +7565,11 @@
         <v>41488</v>
       </c>
       <c r="M31">
-        <f>K31-K30</f>
+        <f t="shared" si="4"/>
         <v>204</v>
       </c>
       <c r="N31">
-        <f>K31/L31</f>
+        <f t="shared" si="1"/>
         <v>0.35622348630929423</v>
       </c>
     </row>
@@ -7582,11 +7581,11 @@
         <v>5043</v>
       </c>
       <c r="C32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="D32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>0.28633749752131665</v>
       </c>
       <c r="F32">
@@ -7596,11 +7595,11 @@
         <v>28170</v>
       </c>
       <c r="H32">
-        <f>F32-F31</f>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
       <c r="I32">
-        <f>F32/G32</f>
+        <f t="shared" si="0"/>
         <v>0.41707490237841677</v>
       </c>
       <c r="K32">
@@ -7610,11 +7609,11 @@
         <v>41707</v>
       </c>
       <c r="M32">
-        <f>K32-K31</f>
+        <f t="shared" si="4"/>
         <v>102</v>
       </c>
       <c r="N32">
-        <f>K32/L32</f>
+        <f t="shared" si="1"/>
         <v>0.35679861893686909</v>
       </c>
     </row>

</xml_diff>